<commit_message>
Populated the paired-end field in all rows
</commit_message>
<xml_diff>
--- a/spreadsheets/new/GSE102596.0.xlsx
+++ b/spreadsheets/new/GSE102596.0.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geryl/PycharmProjects/load-project/spreadsheets/new/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC12C80C-17A3-B744-8E27-E7BC91BDD895}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="31920" windowHeight="17600" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cell_suspension" sheetId="1" r:id="rId1"/>
@@ -17,12 +23,12 @@
     <sheet name="Sequencing_protocol" sheetId="8" r:id="rId8"/>
     <sheet name="Specimen_from_organism" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="865">
   <si>
     <t>CELL_SUSPENSION.BIOMATERIAL_CORE.BIOMATERIAL_ID.USER_FRIENDLY (Required)</t>
   </si>
@@ -2614,13 +2620,16 @@
   </si>
   <si>
     <t>kidney cortex</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2657,6 +2666,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2703,7 +2720,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2735,9 +2752,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2769,6 +2804,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2944,75 +2997,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="73.7109375" customWidth="1"/>
-    <col min="2" max="2" width="71.7109375" customWidth="1"/>
-    <col min="3" max="3" width="71.7109375" customWidth="1"/>
-    <col min="4" max="4" width="47.7109375" customWidth="1"/>
-    <col min="5" max="5" width="61.7109375" customWidth="1"/>
-    <col min="6" max="6" width="106.7109375" customWidth="1"/>
-    <col min="7" max="7" width="176.7109375" customWidth="1"/>
-    <col min="8" max="8" width="171.7109375" customWidth="1"/>
-    <col min="9" max="9" width="134.7109375" customWidth="1"/>
-    <col min="10" max="10" width="57.7109375" customWidth="1"/>
-    <col min="11" max="11" width="85.7109375" customWidth="1"/>
-    <col min="12" max="12" width="69.7109375" customWidth="1"/>
-    <col min="13" max="13" width="58.7109375" customWidth="1"/>
-    <col min="14" max="14" width="141.7109375" customWidth="1"/>
-    <col min="15" max="15" width="70.7109375" customWidth="1"/>
-    <col min="16" max="16" width="57.7109375" customWidth="1"/>
-    <col min="17" max="17" width="54.7109375" customWidth="1"/>
-    <col min="18" max="18" width="68.7109375" customWidth="1"/>
-    <col min="19" max="19" width="62.7109375" customWidth="1"/>
-    <col min="20" max="20" width="81.7109375" customWidth="1"/>
-    <col min="21" max="21" width="61.7109375" customWidth="1"/>
-    <col min="22" max="22" width="195.7109375" customWidth="1"/>
-    <col min="23" max="23" width="62.7109375" customWidth="1"/>
-    <col min="24" max="24" width="150.7109375" customWidth="1"/>
-    <col min="25" max="25" width="78.7109375" customWidth="1"/>
-    <col min="26" max="26" width="64.7109375" customWidth="1"/>
-    <col min="27" max="27" width="58.7109375" customWidth="1"/>
-    <col min="28" max="28" width="141.7109375" customWidth="1"/>
-    <col min="29" max="29" width="163.7109375" customWidth="1"/>
-    <col min="30" max="30" width="58.7109375" customWidth="1"/>
-    <col min="31" max="31" width="141.7109375" customWidth="1"/>
-    <col min="32" max="32" width="52.7109375" customWidth="1"/>
-    <col min="33" max="33" width="63.7109375" customWidth="1"/>
-    <col min="34" max="34" width="59.7109375" customWidth="1"/>
-    <col min="35" max="35" width="108.7109375" customWidth="1"/>
-    <col min="36" max="36" width="108.7109375" customWidth="1"/>
-    <col min="37" max="37" width="69.7109375" customWidth="1"/>
-    <col min="38" max="38" width="58.7109375" customWidth="1"/>
-    <col min="39" max="39" width="141.7109375" customWidth="1"/>
-    <col min="40" max="40" width="117.7109375" customWidth="1"/>
-    <col min="41" max="41" width="80.7109375" customWidth="1"/>
-    <col min="42" max="42" width="73.7109375" customWidth="1"/>
-    <col min="43" max="43" width="71.7109375" customWidth="1"/>
-    <col min="44" max="44" width="32.7109375" customWidth="1"/>
-    <col min="45" max="45" width="67.7109375" customWidth="1"/>
-    <col min="46" max="46" width="41.7109375" customWidth="1"/>
-    <col min="47" max="47" width="84.7109375" customWidth="1"/>
-    <col min="48" max="48" width="104.7109375" customWidth="1"/>
-    <col min="49" max="49" width="104.7109375" customWidth="1"/>
-    <col min="50" max="50" width="104.7109375" customWidth="1"/>
-    <col min="51" max="51" width="88.7109375" customWidth="1"/>
-    <col min="52" max="52" width="69.7109375" customWidth="1"/>
-    <col min="53" max="53" width="58.7109375" customWidth="1"/>
-    <col min="54" max="54" width="141.7109375" customWidth="1"/>
-    <col min="55" max="55" width="67.7109375" customWidth="1"/>
-    <col min="56" max="56" width="58.7109375" customWidth="1"/>
-    <col min="57" max="57" width="141.7109375" customWidth="1"/>
-    <col min="58" max="58" width="79.7109375" customWidth="1"/>
-    <col min="59" max="59" width="175.7109375" customWidth="1"/>
+    <col min="1" max="1" width="73.6640625" customWidth="1"/>
+    <col min="2" max="3" width="71.6640625" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" customWidth="1"/>
+    <col min="5" max="5" width="61.6640625" customWidth="1"/>
+    <col min="6" max="6" width="106.6640625" customWidth="1"/>
+    <col min="7" max="7" width="176.6640625" customWidth="1"/>
+    <col min="8" max="8" width="171.6640625" customWidth="1"/>
+    <col min="9" max="9" width="134.6640625" customWidth="1"/>
+    <col min="10" max="10" width="57.6640625" customWidth="1"/>
+    <col min="11" max="11" width="85.6640625" customWidth="1"/>
+    <col min="12" max="12" width="69.6640625" customWidth="1"/>
+    <col min="13" max="13" width="58.6640625" customWidth="1"/>
+    <col min="14" max="14" width="141.6640625" customWidth="1"/>
+    <col min="15" max="15" width="70.6640625" customWidth="1"/>
+    <col min="16" max="16" width="57.6640625" customWidth="1"/>
+    <col min="17" max="17" width="54.6640625" customWidth="1"/>
+    <col min="18" max="18" width="68.6640625" customWidth="1"/>
+    <col min="19" max="19" width="62.6640625" customWidth="1"/>
+    <col min="20" max="20" width="81.6640625" customWidth="1"/>
+    <col min="21" max="21" width="61.6640625" customWidth="1"/>
+    <col min="22" max="22" width="195.6640625" customWidth="1"/>
+    <col min="23" max="23" width="62.6640625" customWidth="1"/>
+    <col min="24" max="24" width="150.6640625" customWidth="1"/>
+    <col min="25" max="25" width="78.6640625" customWidth="1"/>
+    <col min="26" max="26" width="64.6640625" customWidth="1"/>
+    <col min="27" max="27" width="58.6640625" customWidth="1"/>
+    <col min="28" max="28" width="141.6640625" customWidth="1"/>
+    <col min="29" max="29" width="163.6640625" customWidth="1"/>
+    <col min="30" max="30" width="58.6640625" customWidth="1"/>
+    <col min="31" max="31" width="141.6640625" customWidth="1"/>
+    <col min="32" max="32" width="52.6640625" customWidth="1"/>
+    <col min="33" max="33" width="63.6640625" customWidth="1"/>
+    <col min="34" max="34" width="59.6640625" customWidth="1"/>
+    <col min="35" max="36" width="108.6640625" customWidth="1"/>
+    <col min="37" max="37" width="69.6640625" customWidth="1"/>
+    <col min="38" max="38" width="58.6640625" customWidth="1"/>
+    <col min="39" max="39" width="141.6640625" customWidth="1"/>
+    <col min="40" max="40" width="117.6640625" customWidth="1"/>
+    <col min="41" max="41" width="80.6640625" customWidth="1"/>
+    <col min="42" max="42" width="73.6640625" customWidth="1"/>
+    <col min="43" max="43" width="71.6640625" customWidth="1"/>
+    <col min="44" max="44" width="32.6640625" customWidth="1"/>
+    <col min="45" max="45" width="67.6640625" customWidth="1"/>
+    <col min="46" max="46" width="41.6640625" customWidth="1"/>
+    <col min="47" max="47" width="84.6640625" customWidth="1"/>
+    <col min="48" max="50" width="104.6640625" customWidth="1"/>
+    <col min="51" max="51" width="88.6640625" customWidth="1"/>
+    <col min="52" max="52" width="69.6640625" customWidth="1"/>
+    <col min="53" max="53" width="58.6640625" customWidth="1"/>
+    <col min="54" max="54" width="141.6640625" customWidth="1"/>
+    <col min="55" max="55" width="67.6640625" customWidth="1"/>
+    <col min="56" max="56" width="58.6640625" customWidth="1"/>
+    <col min="57" max="57" width="141.6640625" customWidth="1"/>
+    <col min="58" max="58" width="79.6640625" customWidth="1"/>
+    <col min="59" max="59" width="175.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3191,7 +3242,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:59">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -3370,7 +3421,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:59">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>105</v>
       </c>
@@ -3528,7 +3579,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:59">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>148</v>
       </c>
@@ -3707,12 +3758,12 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:59">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:59">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>208</v>
       </c>
@@ -3741,93 +3792,91 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BY6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="72.7109375" customWidth="1"/>
-    <col min="2" max="2" width="71.7109375" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" customWidth="1"/>
-    <col min="4" max="4" width="46.7109375" customWidth="1"/>
-    <col min="5" max="5" width="61.7109375" customWidth="1"/>
-    <col min="6" max="6" width="62.7109375" customWidth="1"/>
-    <col min="7" max="7" width="176.7109375" customWidth="1"/>
-    <col min="8" max="8" width="171.7109375" customWidth="1"/>
-    <col min="9" max="9" width="134.7109375" customWidth="1"/>
-    <col min="10" max="10" width="46.7109375" customWidth="1"/>
-    <col min="11" max="11" width="103.7109375" customWidth="1"/>
-    <col min="12" max="12" width="58.7109375" customWidth="1"/>
-    <col min="13" max="13" width="141.7109375" customWidth="1"/>
-    <col min="14" max="14" width="42.7109375" customWidth="1"/>
-    <col min="15" max="15" width="58.7109375" customWidth="1"/>
-    <col min="16" max="16" width="141.7109375" customWidth="1"/>
-    <col min="17" max="17" width="62.7109375" customWidth="1"/>
-    <col min="18" max="18" width="58.7109375" customWidth="1"/>
-    <col min="19" max="19" width="141.7109375" customWidth="1"/>
-    <col min="20" max="20" width="65.7109375" customWidth="1"/>
-    <col min="21" max="21" width="221.7109375" customWidth="1"/>
-    <col min="22" max="22" width="106.7109375" customWidth="1"/>
-    <col min="23" max="23" width="69.7109375" customWidth="1"/>
-    <col min="24" max="24" width="58.7109375" customWidth="1"/>
-    <col min="25" max="25" width="141.7109375" customWidth="1"/>
-    <col min="26" max="26" width="77.7109375" customWidth="1"/>
-    <col min="27" max="27" width="58.7109375" customWidth="1"/>
-    <col min="28" max="28" width="141.7109375" customWidth="1"/>
-    <col min="29" max="29" width="82.7109375" customWidth="1"/>
-    <col min="30" max="30" width="58.7109375" customWidth="1"/>
-    <col min="31" max="31" width="141.7109375" customWidth="1"/>
-    <col min="32" max="32" width="134.7109375" customWidth="1"/>
-    <col min="33" max="33" width="90.7109375" customWidth="1"/>
-    <col min="34" max="34" width="52.7109375" customWidth="1"/>
-    <col min="35" max="35" width="143.7109375" customWidth="1"/>
-    <col min="36" max="36" width="136.7109375" customWidth="1"/>
-    <col min="37" max="37" width="147.7109375" customWidth="1"/>
-    <col min="38" max="38" width="155.7109375" customWidth="1"/>
-    <col min="39" max="39" width="172.7109375" customWidth="1"/>
-    <col min="40" max="40" width="129.7109375" customWidth="1"/>
-    <col min="41" max="41" width="137.7109375" customWidth="1"/>
-    <col min="42" max="42" width="74.7109375" customWidth="1"/>
-    <col min="43" max="43" width="89.7109375" customWidth="1"/>
-    <col min="44" max="44" width="174.7109375" customWidth="1"/>
-    <col min="45" max="45" width="154.7109375" customWidth="1"/>
-    <col min="46" max="46" width="69.7109375" customWidth="1"/>
-    <col min="47" max="47" width="58.7109375" customWidth="1"/>
-    <col min="48" max="48" width="141.7109375" customWidth="1"/>
-    <col min="49" max="49" width="109.7109375" customWidth="1"/>
-    <col min="50" max="50" width="69.7109375" customWidth="1"/>
-    <col min="51" max="51" width="58.7109375" customWidth="1"/>
-    <col min="52" max="52" width="141.7109375" customWidth="1"/>
-    <col min="53" max="53" width="106.7109375" customWidth="1"/>
-    <col min="54" max="54" width="69.7109375" customWidth="1"/>
-    <col min="55" max="55" width="58.7109375" customWidth="1"/>
-    <col min="56" max="56" width="141.7109375" customWidth="1"/>
-    <col min="57" max="57" width="108.7109375" customWidth="1"/>
-    <col min="58" max="58" width="69.7109375" customWidth="1"/>
-    <col min="59" max="59" width="58.7109375" customWidth="1"/>
-    <col min="60" max="60" width="141.7109375" customWidth="1"/>
-    <col min="61" max="61" width="117.7109375" customWidth="1"/>
-    <col min="62" max="62" width="32.7109375" customWidth="1"/>
-    <col min="63" max="63" width="67.7109375" customWidth="1"/>
-    <col min="64" max="64" width="41.7109375" customWidth="1"/>
-    <col min="65" max="65" width="84.7109375" customWidth="1"/>
-    <col min="66" max="66" width="104.7109375" customWidth="1"/>
-    <col min="67" max="67" width="104.7109375" customWidth="1"/>
-    <col min="68" max="68" width="104.7109375" customWidth="1"/>
-    <col min="69" max="69" width="88.7109375" customWidth="1"/>
-    <col min="70" max="70" width="69.7109375" customWidth="1"/>
-    <col min="71" max="71" width="58.7109375" customWidth="1"/>
-    <col min="72" max="72" width="141.7109375" customWidth="1"/>
-    <col min="73" max="73" width="67.7109375" customWidth="1"/>
-    <col min="74" max="74" width="58.7109375" customWidth="1"/>
-    <col min="75" max="75" width="141.7109375" customWidth="1"/>
-    <col min="76" max="76" width="79.7109375" customWidth="1"/>
-    <col min="77" max="77" width="175.7109375" customWidth="1"/>
+    <col min="1" max="1" width="72.6640625" customWidth="1"/>
+    <col min="2" max="2" width="71.6640625" customWidth="1"/>
+    <col min="3" max="3" width="70.6640625" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" customWidth="1"/>
+    <col min="5" max="5" width="61.6640625" customWidth="1"/>
+    <col min="6" max="6" width="62.6640625" customWidth="1"/>
+    <col min="7" max="7" width="176.6640625" customWidth="1"/>
+    <col min="8" max="8" width="171.6640625" customWidth="1"/>
+    <col min="9" max="9" width="134.6640625" customWidth="1"/>
+    <col min="10" max="10" width="46.6640625" customWidth="1"/>
+    <col min="11" max="11" width="103.6640625" customWidth="1"/>
+    <col min="12" max="12" width="58.6640625" customWidth="1"/>
+    <col min="13" max="13" width="141.6640625" customWidth="1"/>
+    <col min="14" max="14" width="42.6640625" customWidth="1"/>
+    <col min="15" max="15" width="58.6640625" customWidth="1"/>
+    <col min="16" max="16" width="141.6640625" customWidth="1"/>
+    <col min="17" max="17" width="62.6640625" customWidth="1"/>
+    <col min="18" max="18" width="58.6640625" customWidth="1"/>
+    <col min="19" max="19" width="141.6640625" customWidth="1"/>
+    <col min="20" max="20" width="65.6640625" customWidth="1"/>
+    <col min="21" max="21" width="221.6640625" customWidth="1"/>
+    <col min="22" max="22" width="106.6640625" customWidth="1"/>
+    <col min="23" max="23" width="69.6640625" customWidth="1"/>
+    <col min="24" max="24" width="58.6640625" customWidth="1"/>
+    <col min="25" max="25" width="141.6640625" customWidth="1"/>
+    <col min="26" max="26" width="77.6640625" customWidth="1"/>
+    <col min="27" max="27" width="58.6640625" customWidth="1"/>
+    <col min="28" max="28" width="141.6640625" customWidth="1"/>
+    <col min="29" max="29" width="82.6640625" customWidth="1"/>
+    <col min="30" max="30" width="58.6640625" customWidth="1"/>
+    <col min="31" max="31" width="141.6640625" customWidth="1"/>
+    <col min="32" max="32" width="134.6640625" customWidth="1"/>
+    <col min="33" max="33" width="90.6640625" customWidth="1"/>
+    <col min="34" max="34" width="52.6640625" customWidth="1"/>
+    <col min="35" max="35" width="143.6640625" customWidth="1"/>
+    <col min="36" max="36" width="136.6640625" customWidth="1"/>
+    <col min="37" max="37" width="147.6640625" customWidth="1"/>
+    <col min="38" max="38" width="155.6640625" customWidth="1"/>
+    <col min="39" max="39" width="172.6640625" customWidth="1"/>
+    <col min="40" max="40" width="129.6640625" customWidth="1"/>
+    <col min="41" max="41" width="137.6640625" customWidth="1"/>
+    <col min="42" max="42" width="74.6640625" customWidth="1"/>
+    <col min="43" max="43" width="89.6640625" customWidth="1"/>
+    <col min="44" max="44" width="174.6640625" customWidth="1"/>
+    <col min="45" max="45" width="154.6640625" customWidth="1"/>
+    <col min="46" max="46" width="69.6640625" customWidth="1"/>
+    <col min="47" max="47" width="58.6640625" customWidth="1"/>
+    <col min="48" max="48" width="141.6640625" customWidth="1"/>
+    <col min="49" max="49" width="109.6640625" customWidth="1"/>
+    <col min="50" max="50" width="69.6640625" customWidth="1"/>
+    <col min="51" max="51" width="58.6640625" customWidth="1"/>
+    <col min="52" max="52" width="141.6640625" customWidth="1"/>
+    <col min="53" max="53" width="106.6640625" customWidth="1"/>
+    <col min="54" max="54" width="69.6640625" customWidth="1"/>
+    <col min="55" max="55" width="58.6640625" customWidth="1"/>
+    <col min="56" max="56" width="141.6640625" customWidth="1"/>
+    <col min="57" max="57" width="108.6640625" customWidth="1"/>
+    <col min="58" max="58" width="69.6640625" customWidth="1"/>
+    <col min="59" max="59" width="58.6640625" customWidth="1"/>
+    <col min="60" max="60" width="141.6640625" customWidth="1"/>
+    <col min="61" max="61" width="117.6640625" customWidth="1"/>
+    <col min="62" max="62" width="32.6640625" customWidth="1"/>
+    <col min="63" max="63" width="67.6640625" customWidth="1"/>
+    <col min="64" max="64" width="41.6640625" customWidth="1"/>
+    <col min="65" max="65" width="84.6640625" customWidth="1"/>
+    <col min="66" max="68" width="104.6640625" customWidth="1"/>
+    <col min="69" max="69" width="88.6640625" customWidth="1"/>
+    <col min="70" max="70" width="69.6640625" customWidth="1"/>
+    <col min="71" max="71" width="58.6640625" customWidth="1"/>
+    <col min="72" max="72" width="141.6640625" customWidth="1"/>
+    <col min="73" max="73" width="67.6640625" customWidth="1"/>
+    <col min="74" max="74" width="58.6640625" customWidth="1"/>
+    <col min="75" max="75" width="141.6640625" customWidth="1"/>
+    <col min="76" max="76" width="79.6640625" customWidth="1"/>
+    <col min="77" max="77" width="175.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77">
+    <row r="1" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>215</v>
       </c>
@@ -4060,7 +4109,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:77">
+    <row r="2" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -4293,7 +4342,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:77">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>105</v>
       </c>
@@ -4508,7 +4557,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:77">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>319</v>
       </c>
@@ -4741,12 +4790,12 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:77">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:77">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>380</v>
       </c>
@@ -4769,67 +4818,65 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AY6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="80.7109375" customWidth="1"/>
-    <col min="2" max="2" width="71.7109375" customWidth="1"/>
-    <col min="3" max="3" width="91.7109375" customWidth="1"/>
-    <col min="4" max="4" width="66.7109375" customWidth="1"/>
-    <col min="5" max="5" width="67.7109375" customWidth="1"/>
-    <col min="6" max="6" width="69.7109375" customWidth="1"/>
-    <col min="7" max="7" width="71.7109375" customWidth="1"/>
-    <col min="8" max="8" width="57.7109375" customWidth="1"/>
-    <col min="9" max="9" width="57.7109375" customWidth="1"/>
-    <col min="10" max="10" width="80.7109375" customWidth="1"/>
-    <col min="11" max="11" width="84.7109375" customWidth="1"/>
-    <col min="12" max="12" width="66.7109375" customWidth="1"/>
-    <col min="13" max="13" width="141.7109375" customWidth="1"/>
-    <col min="14" max="14" width="102.7109375" customWidth="1"/>
-    <col min="15" max="15" width="67.7109375" customWidth="1"/>
-    <col min="16" max="16" width="66.7109375" customWidth="1"/>
-    <col min="17" max="17" width="141.7109375" customWidth="1"/>
-    <col min="18" max="18" width="90.7109375" customWidth="1"/>
-    <col min="19" max="19" width="69.7109375" customWidth="1"/>
-    <col min="20" max="20" width="67.7109375" customWidth="1"/>
-    <col min="21" max="21" width="65.7109375" customWidth="1"/>
-    <col min="22" max="22" width="111.7109375" customWidth="1"/>
-    <col min="23" max="23" width="91.7109375" customWidth="1"/>
-    <col min="24" max="24" width="90.7109375" customWidth="1"/>
-    <col min="25" max="25" width="72.7109375" customWidth="1"/>
-    <col min="26" max="26" width="70.7109375" customWidth="1"/>
-    <col min="27" max="27" width="68.7109375" customWidth="1"/>
-    <col min="28" max="28" width="111.7109375" customWidth="1"/>
-    <col min="29" max="29" width="91.7109375" customWidth="1"/>
-    <col min="30" max="30" width="161.7109375" customWidth="1"/>
-    <col min="31" max="31" width="52.7109375" customWidth="1"/>
-    <col min="32" max="32" width="320.7109375" customWidth="1"/>
-    <col min="33" max="33" width="90.7109375" customWidth="1"/>
-    <col min="34" max="34" width="57.7109375" customWidth="1"/>
-    <col min="35" max="35" width="55.7109375" customWidth="1"/>
-    <col min="36" max="36" width="53.7109375" customWidth="1"/>
-    <col min="37" max="37" width="111.7109375" customWidth="1"/>
-    <col min="38" max="38" width="91.7109375" customWidth="1"/>
-    <col min="39" max="39" width="47.7109375" customWidth="1"/>
-    <col min="40" max="40" width="71.7109375" customWidth="1"/>
-    <col min="41" max="41" width="56.7109375" customWidth="1"/>
-    <col min="42" max="42" width="56.7109375" customWidth="1"/>
-    <col min="43" max="43" width="80.7109375" customWidth="1"/>
-    <col min="44" max="44" width="67.7109375" customWidth="1"/>
-    <col min="45" max="45" width="70.7109375" customWidth="1"/>
-    <col min="46" max="46" width="141.7109375" customWidth="1"/>
-    <col min="47" max="47" width="68.7109375" customWidth="1"/>
-    <col min="48" max="48" width="72.7109375" customWidth="1"/>
-    <col min="49" max="49" width="141.7109375" customWidth="1"/>
-    <col min="50" max="50" width="56.7109375" customWidth="1"/>
-    <col min="51" max="51" width="74.7109375" customWidth="1"/>
+    <col min="1" max="1" width="80.6640625" customWidth="1"/>
+    <col min="2" max="2" width="71.6640625" customWidth="1"/>
+    <col min="3" max="3" width="91.6640625" customWidth="1"/>
+    <col min="4" max="4" width="66.6640625" customWidth="1"/>
+    <col min="5" max="5" width="67.6640625" customWidth="1"/>
+    <col min="6" max="6" width="69.6640625" customWidth="1"/>
+    <col min="7" max="7" width="71.6640625" customWidth="1"/>
+    <col min="8" max="9" width="57.6640625" customWidth="1"/>
+    <col min="10" max="10" width="80.6640625" customWidth="1"/>
+    <col min="11" max="11" width="84.6640625" customWidth="1"/>
+    <col min="12" max="12" width="66.6640625" customWidth="1"/>
+    <col min="13" max="13" width="141.6640625" customWidth="1"/>
+    <col min="14" max="14" width="102.6640625" customWidth="1"/>
+    <col min="15" max="15" width="67.6640625" customWidth="1"/>
+    <col min="16" max="16" width="66.6640625" customWidth="1"/>
+    <col min="17" max="17" width="141.6640625" customWidth="1"/>
+    <col min="18" max="18" width="90.6640625" customWidth="1"/>
+    <col min="19" max="19" width="69.6640625" customWidth="1"/>
+    <col min="20" max="20" width="67.6640625" customWidth="1"/>
+    <col min="21" max="21" width="65.6640625" customWidth="1"/>
+    <col min="22" max="22" width="111.6640625" customWidth="1"/>
+    <col min="23" max="23" width="91.6640625" customWidth="1"/>
+    <col min="24" max="24" width="90.6640625" customWidth="1"/>
+    <col min="25" max="25" width="72.6640625" customWidth="1"/>
+    <col min="26" max="26" width="70.6640625" customWidth="1"/>
+    <col min="27" max="27" width="68.6640625" customWidth="1"/>
+    <col min="28" max="28" width="111.6640625" customWidth="1"/>
+    <col min="29" max="29" width="91.6640625" customWidth="1"/>
+    <col min="30" max="30" width="161.6640625" customWidth="1"/>
+    <col min="31" max="31" width="52.6640625" customWidth="1"/>
+    <col min="32" max="32" width="320.6640625" customWidth="1"/>
+    <col min="33" max="33" width="90.6640625" customWidth="1"/>
+    <col min="34" max="34" width="57.6640625" customWidth="1"/>
+    <col min="35" max="35" width="55.6640625" customWidth="1"/>
+    <col min="36" max="36" width="53.6640625" customWidth="1"/>
+    <col min="37" max="37" width="111.6640625" customWidth="1"/>
+    <col min="38" max="38" width="91.6640625" customWidth="1"/>
+    <col min="39" max="39" width="47.6640625" customWidth="1"/>
+    <col min="40" max="40" width="71.6640625" customWidth="1"/>
+    <col min="41" max="42" width="56.6640625" customWidth="1"/>
+    <col min="43" max="43" width="80.6640625" customWidth="1"/>
+    <col min="44" max="44" width="67.6640625" customWidth="1"/>
+    <col min="45" max="45" width="70.6640625" customWidth="1"/>
+    <col min="46" max="46" width="141.6640625" customWidth="1"/>
+    <col min="47" max="47" width="68.6640625" customWidth="1"/>
+    <col min="48" max="48" width="72.6640625" customWidth="1"/>
+    <col min="49" max="49" width="141.6640625" customWidth="1"/>
+    <col min="50" max="50" width="56.6640625" customWidth="1"/>
+    <col min="51" max="51" width="74.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>384</v>
       </c>
@@ -4984,7 +5031,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="2" spans="1:51">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -5139,7 +5186,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="3" spans="1:51">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -5288,7 +5335,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="4" spans="1:51">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>485</v>
       </c>
@@ -5443,12 +5490,12 @@
         <v>535</v>
       </c>
     </row>
-    <row r="5" spans="1:51">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:51">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>536</v>
       </c>
@@ -5465,25 +5512,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="162.7109375" customWidth="1"/>
-    <col min="2" max="2" width="153.7109375" customWidth="1"/>
-    <col min="3" max="3" width="178.7109375" customWidth="1"/>
-    <col min="4" max="4" width="135.7109375" customWidth="1"/>
-    <col min="5" max="5" width="171.7109375" customWidth="1"/>
-    <col min="6" max="6" width="99.7109375" customWidth="1"/>
-    <col min="7" max="7" width="99.7109375" customWidth="1"/>
-    <col min="8" max="8" width="174.7109375" customWidth="1"/>
-    <col min="9" max="9" width="75.7109375" customWidth="1"/>
+    <col min="1" max="1" width="162.6640625" customWidth="1"/>
+    <col min="2" max="2" width="153.6640625" customWidth="1"/>
+    <col min="3" max="3" width="178.6640625" customWidth="1"/>
+    <col min="4" max="4" width="135.6640625" customWidth="1"/>
+    <col min="5" max="5" width="171.6640625" customWidth="1"/>
+    <col min="6" max="7" width="99.6640625" customWidth="1"/>
+    <col min="8" max="8" width="174.6640625" customWidth="1"/>
+    <col min="9" max="9" width="75.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>539</v>
       </c>
@@ -5512,7 +5558,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>548</v>
       </c>
@@ -5541,7 +5587,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>557</v>
       </c>
@@ -5570,7 +5616,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>566</v>
       </c>
@@ -5599,12 +5645,12 @@
         <v>574</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>575</v>
       </c>
@@ -5630,28 +5676,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="103.7109375" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1"/>
-    <col min="3" max="3" width="57.7109375" customWidth="1"/>
-    <col min="4" max="4" width="54.7109375" customWidth="1"/>
-    <col min="5" max="5" width="75.7109375" customWidth="1"/>
-    <col min="6" max="6" width="127.7109375" customWidth="1"/>
-    <col min="7" max="7" width="36.7109375" customWidth="1"/>
-    <col min="8" max="8" width="70.7109375" customWidth="1"/>
-    <col min="9" max="9" width="64.7109375" customWidth="1"/>
-    <col min="10" max="10" width="58.7109375" customWidth="1"/>
-    <col min="11" max="11" width="141.7109375" customWidth="1"/>
-    <col min="12" max="12" width="51.7109375" customWidth="1"/>
+    <col min="1" max="1" width="103.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
+    <col min="3" max="3" width="57.6640625" customWidth="1"/>
+    <col min="4" max="4" width="54.6640625" customWidth="1"/>
+    <col min="5" max="5" width="75.6640625" customWidth="1"/>
+    <col min="6" max="6" width="127.6640625" customWidth="1"/>
+    <col min="7" max="7" width="36.6640625" customWidth="1"/>
+    <col min="8" max="8" width="70.6640625" customWidth="1"/>
+    <col min="9" max="9" width="64.6640625" customWidth="1"/>
+    <col min="10" max="10" width="58.6640625" customWidth="1"/>
+    <col min="11" max="11" width="141.6640625" customWidth="1"/>
+    <col min="12" max="12" width="51.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>581</v>
       </c>
@@ -5689,7 +5735,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>593</v>
       </c>
@@ -5727,7 +5773,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>603</v>
       </c>
@@ -5765,7 +5811,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>614</v>
       </c>
@@ -5803,12 +5849,12 @@
         <v>625</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>626</v>
       </c>
@@ -5828,27 +5874,27 @@
         <v>631</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>636</v>
       </c>
@@ -5859,21 +5905,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="67.7109375" customWidth="1"/>
-    <col min="2" max="2" width="55.7109375" customWidth="1"/>
-    <col min="3" max="3" width="68.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" customWidth="1"/>
-    <col min="5" max="5" width="68.7109375" customWidth="1"/>
+    <col min="1" max="1" width="67.6640625" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="68.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" customWidth="1"/>
+    <col min="5" max="5" width="68.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>637</v>
       </c>
@@ -5890,7 +5936,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>641</v>
       </c>
@@ -5907,7 +5953,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>646</v>
       </c>
@@ -5924,7 +5970,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>651</v>
       </c>
@@ -5941,12 +5987,12 @@
         <v>655</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>656</v>
       </c>
@@ -5957,46 +6003,44 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AD9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="85.7109375" customWidth="1"/>
-    <col min="2" max="2" width="94.7109375" customWidth="1"/>
-    <col min="3" max="3" width="53.7109375" customWidth="1"/>
-    <col min="4" max="4" width="58.7109375" customWidth="1"/>
-    <col min="5" max="5" width="141.7109375" customWidth="1"/>
-    <col min="6" max="6" width="47.7109375" customWidth="1"/>
-    <col min="7" max="7" width="117.7109375" customWidth="1"/>
-    <col min="8" max="8" width="44.7109375" customWidth="1"/>
-    <col min="9" max="9" width="61.7109375" customWidth="1"/>
-    <col min="10" max="10" width="168.7109375" customWidth="1"/>
-    <col min="11" max="11" width="156.7109375" customWidth="1"/>
-    <col min="12" max="12" width="73.7109375" customWidth="1"/>
-    <col min="13" max="13" width="80.7109375" customWidth="1"/>
-    <col min="14" max="14" width="71.7109375" customWidth="1"/>
-    <col min="15" max="15" width="32.7109375" customWidth="1"/>
-    <col min="16" max="16" width="67.7109375" customWidth="1"/>
-    <col min="17" max="17" width="41.7109375" customWidth="1"/>
-    <col min="18" max="18" width="84.7109375" customWidth="1"/>
-    <col min="19" max="19" width="104.7109375" customWidth="1"/>
-    <col min="20" max="20" width="104.7109375" customWidth="1"/>
-    <col min="21" max="21" width="104.7109375" customWidth="1"/>
-    <col min="22" max="22" width="88.7109375" customWidth="1"/>
-    <col min="23" max="23" width="69.7109375" customWidth="1"/>
-    <col min="24" max="24" width="58.7109375" customWidth="1"/>
-    <col min="25" max="25" width="141.7109375" customWidth="1"/>
-    <col min="26" max="26" width="67.7109375" customWidth="1"/>
-    <col min="27" max="27" width="58.7109375" customWidth="1"/>
-    <col min="28" max="28" width="141.7109375" customWidth="1"/>
-    <col min="29" max="29" width="79.7109375" customWidth="1"/>
-    <col min="30" max="30" width="175.7109375" customWidth="1"/>
+    <col min="1" max="1" width="85.6640625" customWidth="1"/>
+    <col min="2" max="2" width="94.6640625" customWidth="1"/>
+    <col min="3" max="3" width="53.6640625" customWidth="1"/>
+    <col min="4" max="4" width="58.6640625" customWidth="1"/>
+    <col min="5" max="5" width="141.6640625" customWidth="1"/>
+    <col min="6" max="6" width="47.6640625" customWidth="1"/>
+    <col min="7" max="7" width="117.6640625" customWidth="1"/>
+    <col min="8" max="8" width="44.6640625" customWidth="1"/>
+    <col min="9" max="9" width="61.6640625" customWidth="1"/>
+    <col min="10" max="10" width="168.6640625" customWidth="1"/>
+    <col min="11" max="11" width="156.6640625" customWidth="1"/>
+    <col min="12" max="12" width="73.6640625" customWidth="1"/>
+    <col min="13" max="13" width="80.6640625" customWidth="1"/>
+    <col min="14" max="14" width="71.6640625" customWidth="1"/>
+    <col min="15" max="15" width="32.6640625" customWidth="1"/>
+    <col min="16" max="16" width="67.6640625" customWidth="1"/>
+    <col min="17" max="17" width="41.6640625" customWidth="1"/>
+    <col min="18" max="18" width="84.6640625" customWidth="1"/>
+    <col min="19" max="21" width="104.6640625" customWidth="1"/>
+    <col min="22" max="22" width="88.6640625" customWidth="1"/>
+    <col min="23" max="23" width="69.6640625" customWidth="1"/>
+    <col min="24" max="24" width="58.6640625" customWidth="1"/>
+    <col min="25" max="25" width="141.6640625" customWidth="1"/>
+    <col min="26" max="26" width="67.6640625" customWidth="1"/>
+    <col min="27" max="27" width="58.6640625" customWidth="1"/>
+    <col min="28" max="28" width="141.6640625" customWidth="1"/>
+    <col min="29" max="29" width="79.6640625" customWidth="1"/>
+    <col min="30" max="30" width="175.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>657</v>
       </c>
@@ -6088,7 +6132,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>669</v>
       </c>
@@ -6180,7 +6224,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>678</v>
       </c>
@@ -6260,7 +6304,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>688</v>
       </c>
@@ -6352,12 +6396,12 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>700</v>
       </c>
@@ -6380,7 +6424,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>705</v>
       </c>
@@ -6403,7 +6447,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>707</v>
       </c>
@@ -6426,7 +6470,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>709</v>
       </c>
@@ -6455,34 +6499,36 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="J4" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="71.7109375" customWidth="1"/>
-    <col min="2" max="2" width="62.7109375" customWidth="1"/>
-    <col min="3" max="3" width="91.7109375" customWidth="1"/>
-    <col min="4" max="4" width="66.7109375" customWidth="1"/>
-    <col min="5" max="5" width="67.7109375" customWidth="1"/>
-    <col min="6" max="6" width="69.7109375" customWidth="1"/>
-    <col min="7" max="7" width="70.7109375" customWidth="1"/>
-    <col min="8" max="8" width="59.7109375" customWidth="1"/>
-    <col min="9" max="9" width="141.7109375" customWidth="1"/>
-    <col min="10" max="10" width="59.7109375" customWidth="1"/>
-    <col min="11" max="11" width="76.7109375" customWidth="1"/>
-    <col min="12" max="12" width="91.7109375" customWidth="1"/>
-    <col min="13" max="13" width="58.7109375" customWidth="1"/>
-    <col min="14" max="14" width="141.7109375" customWidth="1"/>
-    <col min="15" max="15" width="62.7109375" customWidth="1"/>
-    <col min="16" max="16" width="50.7109375" customWidth="1"/>
-    <col min="17" max="17" width="56.7109375" customWidth="1"/>
-    <col min="18" max="18" width="99.7109375" customWidth="1"/>
+    <col min="1" max="1" width="71.6640625" customWidth="1"/>
+    <col min="2" max="2" width="62.6640625" customWidth="1"/>
+    <col min="3" max="3" width="91.6640625" customWidth="1"/>
+    <col min="4" max="4" width="66.6640625" customWidth="1"/>
+    <col min="5" max="5" width="67.6640625" customWidth="1"/>
+    <col min="6" max="6" width="69.6640625" customWidth="1"/>
+    <col min="7" max="7" width="70.6640625" customWidth="1"/>
+    <col min="8" max="8" width="59.6640625" customWidth="1"/>
+    <col min="9" max="9" width="141.6640625" customWidth="1"/>
+    <col min="10" max="10" width="59.6640625" customWidth="1"/>
+    <col min="11" max="11" width="76.6640625" customWidth="1"/>
+    <col min="12" max="12" width="91.6640625" customWidth="1"/>
+    <col min="13" max="13" width="58.6640625" customWidth="1"/>
+    <col min="14" max="14" width="141.6640625" customWidth="1"/>
+    <col min="15" max="15" width="62.6640625" customWidth="1"/>
+    <col min="16" max="16" width="50.6640625" customWidth="1"/>
+    <col min="17" max="17" width="56.6640625" customWidth="1"/>
+    <col min="18" max="18" width="99.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>668</v>
       </c>
@@ -6538,7 +6584,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -6594,7 +6640,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -6644,7 +6690,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>699</v>
       </c>
@@ -6700,12 +6746,12 @@
         <v>755</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>704</v>
       </c>
@@ -6714,6 +6760,9 @@
       </c>
       <c r="G6" t="s">
         <v>756</v>
+      </c>
+      <c r="K6" t="s">
+        <v>864</v>
       </c>
     </row>
   </sheetData>
@@ -6722,76 +6771,73 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:BH6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="80.7109375" customWidth="1"/>
-    <col min="2" max="2" width="71.7109375" customWidth="1"/>
-    <col min="3" max="3" width="78.7109375" customWidth="1"/>
-    <col min="4" max="4" width="54.7109375" customWidth="1"/>
-    <col min="5" max="5" width="61.7109375" customWidth="1"/>
-    <col min="6" max="6" width="62.7109375" customWidth="1"/>
-    <col min="7" max="7" width="176.7109375" customWidth="1"/>
-    <col min="8" max="8" width="171.7109375" customWidth="1"/>
-    <col min="9" max="9" width="134.7109375" customWidth="1"/>
-    <col min="10" max="10" width="62.7109375" customWidth="1"/>
-    <col min="11" max="11" width="58.7109375" customWidth="1"/>
-    <col min="12" max="12" width="141.7109375" customWidth="1"/>
-    <col min="13" max="13" width="69.7109375" customWidth="1"/>
-    <col min="14" max="14" width="58.7109375" customWidth="1"/>
-    <col min="15" max="15" width="141.7109375" customWidth="1"/>
-    <col min="16" max="16" width="96.7109375" customWidth="1"/>
-    <col min="17" max="17" width="58.7109375" customWidth="1"/>
-    <col min="18" max="18" width="141.7109375" customWidth="1"/>
-    <col min="19" max="19" width="81.7109375" customWidth="1"/>
-    <col min="20" max="20" width="58.7109375" customWidth="1"/>
-    <col min="21" max="21" width="141.7109375" customWidth="1"/>
-    <col min="22" max="22" width="57.7109375" customWidth="1"/>
-    <col min="23" max="23" width="76.7109375" customWidth="1"/>
-    <col min="24" max="24" width="80.7109375" customWidth="1"/>
-    <col min="25" max="25" width="62.7109375" customWidth="1"/>
-    <col min="26" max="26" width="121.7109375" customWidth="1"/>
-    <col min="27" max="27" width="97.7109375" customWidth="1"/>
-    <col min="28" max="28" width="86.7109375" customWidth="1"/>
-    <col min="29" max="29" width="99.7109375" customWidth="1"/>
-    <col min="30" max="30" width="101.7109375" customWidth="1"/>
-    <col min="31" max="31" width="69.7109375" customWidth="1"/>
-    <col min="32" max="32" width="69.7109375" customWidth="1"/>
-    <col min="33" max="33" width="71.7109375" customWidth="1"/>
-    <col min="34" max="34" width="141.7109375" customWidth="1"/>
-    <col min="35" max="35" width="158.7109375" customWidth="1"/>
-    <col min="36" max="36" width="136.7109375" customWidth="1"/>
-    <col min="37" max="37" width="90.7109375" customWidth="1"/>
-    <col min="38" max="38" width="57.7109375" customWidth="1"/>
-    <col min="39" max="39" width="55.7109375" customWidth="1"/>
-    <col min="40" max="40" width="53.7109375" customWidth="1"/>
-    <col min="41" max="41" width="111.7109375" customWidth="1"/>
-    <col min="42" max="42" width="91.7109375" customWidth="1"/>
-    <col min="43" max="43" width="72.7109375" customWidth="1"/>
-    <col min="44" max="44" width="71.7109375" customWidth="1"/>
-    <col min="45" max="45" width="32.7109375" customWidth="1"/>
-    <col min="46" max="46" width="67.7109375" customWidth="1"/>
-    <col min="47" max="47" width="41.7109375" customWidth="1"/>
-    <col min="48" max="48" width="84.7109375" customWidth="1"/>
-    <col min="49" max="49" width="104.7109375" customWidth="1"/>
-    <col min="50" max="50" width="104.7109375" customWidth="1"/>
-    <col min="51" max="51" width="104.7109375" customWidth="1"/>
-    <col min="52" max="52" width="88.7109375" customWidth="1"/>
-    <col min="53" max="53" width="69.7109375" customWidth="1"/>
-    <col min="54" max="54" width="58.7109375" customWidth="1"/>
-    <col min="55" max="55" width="141.7109375" customWidth="1"/>
-    <col min="56" max="56" width="67.7109375" customWidth="1"/>
-    <col min="57" max="57" width="58.7109375" customWidth="1"/>
-    <col min="58" max="58" width="141.7109375" customWidth="1"/>
-    <col min="59" max="59" width="79.7109375" customWidth="1"/>
-    <col min="60" max="60" width="175.7109375" customWidth="1"/>
+    <col min="1" max="1" width="80.6640625" customWidth="1"/>
+    <col min="2" max="2" width="71.6640625" customWidth="1"/>
+    <col min="3" max="3" width="78.6640625" customWidth="1"/>
+    <col min="4" max="4" width="54.6640625" customWidth="1"/>
+    <col min="5" max="5" width="61.6640625" customWidth="1"/>
+    <col min="6" max="6" width="62.6640625" customWidth="1"/>
+    <col min="7" max="7" width="176.6640625" customWidth="1"/>
+    <col min="8" max="8" width="171.6640625" customWidth="1"/>
+    <col min="9" max="9" width="134.6640625" customWidth="1"/>
+    <col min="10" max="10" width="62.6640625" customWidth="1"/>
+    <col min="11" max="11" width="58.6640625" customWidth="1"/>
+    <col min="12" max="12" width="141.6640625" customWidth="1"/>
+    <col min="13" max="13" width="69.6640625" customWidth="1"/>
+    <col min="14" max="14" width="58.6640625" customWidth="1"/>
+    <col min="15" max="15" width="141.6640625" customWidth="1"/>
+    <col min="16" max="16" width="96.6640625" customWidth="1"/>
+    <col min="17" max="17" width="58.6640625" customWidth="1"/>
+    <col min="18" max="18" width="141.6640625" customWidth="1"/>
+    <col min="19" max="19" width="81.6640625" customWidth="1"/>
+    <col min="20" max="20" width="58.6640625" customWidth="1"/>
+    <col min="21" max="21" width="141.6640625" customWidth="1"/>
+    <col min="22" max="22" width="57.6640625" customWidth="1"/>
+    <col min="23" max="23" width="76.6640625" customWidth="1"/>
+    <col min="24" max="24" width="80.6640625" customWidth="1"/>
+    <col min="25" max="25" width="62.6640625" customWidth="1"/>
+    <col min="26" max="26" width="121.6640625" customWidth="1"/>
+    <col min="27" max="27" width="97.6640625" customWidth="1"/>
+    <col min="28" max="28" width="86.6640625" customWidth="1"/>
+    <col min="29" max="29" width="99.6640625" customWidth="1"/>
+    <col min="30" max="30" width="101.6640625" customWidth="1"/>
+    <col min="31" max="32" width="69.6640625" customWidth="1"/>
+    <col min="33" max="33" width="71.6640625" customWidth="1"/>
+    <col min="34" max="34" width="141.6640625" customWidth="1"/>
+    <col min="35" max="35" width="158.6640625" customWidth="1"/>
+    <col min="36" max="36" width="136.6640625" customWidth="1"/>
+    <col min="37" max="37" width="90.6640625" customWidth="1"/>
+    <col min="38" max="38" width="57.6640625" customWidth="1"/>
+    <col min="39" max="39" width="55.6640625" customWidth="1"/>
+    <col min="40" max="40" width="53.6640625" customWidth="1"/>
+    <col min="41" max="41" width="111.6640625" customWidth="1"/>
+    <col min="42" max="42" width="91.6640625" customWidth="1"/>
+    <col min="43" max="43" width="72.6640625" customWidth="1"/>
+    <col min="44" max="44" width="71.6640625" customWidth="1"/>
+    <col min="45" max="45" width="32.6640625" customWidth="1"/>
+    <col min="46" max="46" width="67.6640625" customWidth="1"/>
+    <col min="47" max="47" width="41.6640625" customWidth="1"/>
+    <col min="48" max="48" width="84.6640625" customWidth="1"/>
+    <col min="49" max="51" width="104.6640625" customWidth="1"/>
+    <col min="52" max="52" width="88.6640625" customWidth="1"/>
+    <col min="53" max="53" width="69.6640625" customWidth="1"/>
+    <col min="54" max="54" width="58.6640625" customWidth="1"/>
+    <col min="55" max="55" width="141.6640625" customWidth="1"/>
+    <col min="56" max="56" width="67.6640625" customWidth="1"/>
+    <col min="57" max="57" width="58.6640625" customWidth="1"/>
+    <col min="58" max="58" width="141.6640625" customWidth="1"/>
+    <col min="59" max="59" width="79.6640625" customWidth="1"/>
+    <col min="60" max="60" width="175.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -6973,7 +7019,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:60">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -7155,7 +7201,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:60">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>105</v>
       </c>
@@ -7316,7 +7362,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:60">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>188</v>
       </c>
@@ -7498,12 +7544,12 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:60">
+    <row r="5" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:60">
+    <row r="6" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>214</v>
       </c>

</xml_diff>